<commit_message>
Update IP - EX 47 - Subtotal (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 47 - Subtotal (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 47 - Subtotal (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83AFCC55-7152-443D-BDC3-BE1200EC0D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0B1263-CECC-401E-A263-437F2D83A25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>CONCEITO</t>
   </si>
@@ -1117,7 +1117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:Q25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1429,10 @@
       <c r="I10" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="19"/>
+      <c r="J10" s="19">
+        <f>SUM(B10:B20)</f>
+        <v>90</v>
+      </c>
       <c r="N10" s="34" t="s">
         <v>2</v>
       </c>
@@ -1459,7 +1462,10 @@
       <c r="I11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="19"/>
+      <c r="J11" s="19">
+        <f>SUBTOTAL(109,B10:B20)</f>
+        <v>90</v>
+      </c>
       <c r="N11" s="32" t="s">
         <v>3</v>
       </c>
@@ -1599,7 +1605,9 @@
       <c r="H16" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="19">
+        <v>9</v>
+      </c>
       <c r="N16" s="32" t="s">
         <v>8</v>
       </c>
@@ -1629,7 +1637,10 @@
       <c r="H17" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="19"/>
+      <c r="J17" s="19">
+        <f>SUBTOTAL(J16,B10:F20)</f>
+        <v>860</v>
+      </c>
       <c r="N17" s="32" t="s">
         <v>9</v>
       </c>
@@ -1726,7 +1737,9 @@
       <c r="H23" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="46"/>
+      <c r="I23" s="46" t="s">
+        <v>7</v>
+      </c>
       <c r="J23" s="47"/>
     </row>
     <row r="24" spans="2:16" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1736,13 +1749,21 @@
       <c r="H25" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="19"/>
+      <c r="J25" s="19">
+        <f>SUBTOTAL(VLOOKUP($I$23,$N$10:$P$19,3,FALSE),B10:F20)</f>
+        <v>7.8772142950731663</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:Q6"/>
     <mergeCell ref="I23:J23"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I23:J23" xr:uid="{111FBB5B-3524-4FEC-A355-B453C288A044}">
+      <formula1>$N$11:$N$19</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>